<commit_message>
Esqueleto de los metodos post realizado
Ahora es capaz de reconocer metodos post y realizar el esqueleto concreto de dichos metodos (sin funcionalidad)
</commit_message>
<xml_diff>
--- a/TFG/target/excel/excel.xlsx
+++ b/TFG/target/excel/excel.xlsx
@@ -13,9 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>configuracion</t>
+  </si>
+  <si>
+    <t>post</t>
   </si>
   <si>
     <t>get</t>
@@ -24,13 +27,22 @@
     <t>entrada</t>
   </si>
   <si>
+    <t>valor1</t>
+  </si>
+  <si>
     <t>restando1</t>
+  </si>
+  <si>
+    <t>valor2</t>
   </si>
   <si>
     <t>sumando1</t>
   </si>
   <si>
-    <t>valor1</t>
+    <t>valor3</t>
+  </si>
+  <si>
+    <t>valor4</t>
   </si>
   <si>
     <t>sumando2</t>
@@ -39,26 +51,17 @@
     <t>salida</t>
   </si>
   <si>
-    <t>valor2</t>
-  </si>
-  <si>
-    <t>valor3</t>
-  </si>
-  <si>
-    <t>valor4</t>
+    <t>restando2</t>
   </si>
   <si>
     <t>gastoTotal</t>
-  </si>
-  <si>
-    <t>restando2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -70,14 +73,11 @@
     </font>
     <font>
       <sz val="10.0"/>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="10.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -181,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -191,46 +191,40 @@
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -463,55 +457,55 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C1" s="3"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="9"/>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12">
+        <f>C2+C3</f>
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="13">
-        <f>C2+C3+2</f>
-        <v>4</v>
-      </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="D5" s="15"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="D6" s="15"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="E7" s="17"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" ht="12.75" customHeight="1"/>
     <row r="9" ht="12.0" customHeight="1"/>
@@ -520,13 +514,13 @@
     <row r="12" ht="12.75" customHeight="1"/>
     <row r="13" ht="12.75" customHeight="1"/>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="D14" s="17"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="D15" s="17"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="D16" s="17"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
     <row r="18" ht="12.75" customHeight="1"/>
@@ -1537,48 +1531,48 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8">
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7">
         <v>2.0</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>1.0</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="16">
+      <c r="B4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="13">
         <f>C2-C3</f>
         <v>1</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="15"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1605,57 +1599,57 @@
       <c r="C1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
+      <c r="A2" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="7">
         <v>5.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="s">
-        <v>2</v>
+      <c r="A3" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
-        <v>2</v>
+      <c r="A4" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>2</v>
+      <c r="A5" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="8">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="16">
+      <c r="B6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="13">
         <f>(C2/4)*C3+C4*C5</f>
         <v>3.5</v>
       </c>

</xml_diff>

<commit_message>
Lectura de los body
Ahora se leen y almacenan los bodys correctamente
</commit_message>
<xml_diff>
--- a/TFG/target/excel/excel.xlsx
+++ b/TFG/target/excel/excel.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="suma" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="resta" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="compleja" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="post" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>configuracion</t>
   </si>
@@ -33,35 +34,47 @@
     <t>restando1</t>
   </si>
   <si>
+    <t>sumando1</t>
+  </si>
+  <si>
+    <t>sumando2</t>
+  </si>
+  <si>
     <t>valor2</t>
   </si>
   <si>
-    <t>sumando1</t>
+    <t>restando2</t>
   </si>
   <si>
     <t>valor3</t>
   </si>
   <si>
+    <t>salida</t>
+  </si>
+  <si>
     <t>valor4</t>
   </si>
   <si>
-    <t>sumando2</t>
+    <t>gastoTotal</t>
   </si>
   <si>
-    <t>salida</t>
+    <t>body</t>
   </si>
   <si>
-    <t>restando2</t>
+    <t>nombre</t>
   </si>
   <si>
-    <t>gastoTotal</t>
+    <t>tomas</t>
+  </si>
+  <si>
+    <t>dinero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -94,6 +107,10 @@
       <color rgb="FF6666FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <name val="Arial"/>
+    </font>
+    <font/>
   </fonts>
   <fills count="9">
     <fill>
@@ -181,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -191,10 +208,10 @@
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -210,20 +227,32 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="8" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -242,6 +271,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -457,17 +490,17 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="6">
         <v>1.0</v>
@@ -478,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6">
         <v>1.0</v>
@@ -486,7 +519,7 @@
       <c r="D3" s="9"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -496,16 +529,16 @@
         <f>C2+C3</f>
         <v>2</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="D5" s="14"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="D6" s="14"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="E7" s="16"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" ht="12.75" customHeight="1"/>
     <row r="9" ht="12.0" customHeight="1"/>
@@ -514,13 +547,13 @@
     <row r="12" ht="12.75" customHeight="1"/>
     <row r="13" ht="12.75" customHeight="1"/>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="D14" s="16"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="D15" s="16"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="D16" s="16"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
     <row r="18" ht="12.75" customHeight="1"/>
@@ -1531,11 +1564,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
@@ -1554,25 +1587,25 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="7">
         <v>1.0</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="14">
         <f>C2-C3</f>
         <v>1</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="16"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1596,7 +1629,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
@@ -1614,7 +1647,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="7">
         <v>2.0</v>
@@ -1625,7 +1658,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7">
         <v>1.0</v>
@@ -1636,22 +1669,90 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7">
         <v>1.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="14">
         <f>(C2/4)*C3+C4*C5</f>
         <v>3.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="19">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="18">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="20">
+        <v>5.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generacion de metodos POST modificados
*Se crean clases especificas dependiendo del json de entrada.
*Se crean las cabeceras dependiendo de la clase concreta BODY.
* Se modifica astah
* Se crea fichero de tareas
</commit_message>
<xml_diff>
--- a/TFG/target/excel/excel.xlsx
+++ b/TFG/target/excel/excel.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="resta" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="compleja" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="post" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="post2" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
   <si>
     <t>configuracion</t>
   </si>
@@ -28,13 +29,13 @@
     <t>entrada</t>
   </si>
   <si>
+    <t>sumando1</t>
+  </si>
+  <si>
     <t>valor1</t>
   </si>
   <si>
     <t>restando1</t>
-  </si>
-  <si>
-    <t>sumando1</t>
   </si>
   <si>
     <t>sumando2</t>
@@ -74,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -82,10 +83,6 @@
     </font>
     <font>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -107,10 +104,6 @@
       <color rgb="FF6666FF"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <name val="Arial"/>
-    </font>
-    <font/>
   </fonts>
   <fills count="9">
     <fill>
@@ -198,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -208,51 +201,36 @@
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -275,6 +253,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -490,52 +472,52 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1.0</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <f>C2+C3</f>
         <v>2</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="D5" s="13"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="D6" s="13"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="E7" s="15"/>
@@ -1564,48 +1546,48 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7">
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6">
         <v>2.0</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>1.0</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <f>C2-C3</f>
         <v>1</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="13"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1629,60 +1611,60 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7">
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6">
         <v>5.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <f>(C2/4)*C3+C4*C5</f>
         <v>3.5</v>
       </c>
@@ -1706,52 +1688,109 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="19">
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6">
         <v>5.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="5">
         <v>2.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="11">
+        <v>5.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="11">
         <v>5.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arrays en los metodos POST
* Se reconocen los arrays en los metodos POST
</commit_message>
<xml_diff>
--- a/TFG/target/excel/excel.xlsx
+++ b/TFG/target/excel/excel.xlsx
@@ -15,36 +15,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>configuracion</t>
+  </si>
+  <si>
+    <t>get</t>
   </si>
   <si>
     <t>post</t>
   </si>
   <si>
-    <t>get</t>
+    <t>entrada</t>
   </si>
   <si>
-    <t>entrada</t>
+    <t>restando1</t>
   </si>
   <si>
     <t>sumando1</t>
   </si>
   <si>
+    <t>sumando2</t>
+  </si>
+  <si>
     <t>valor1</t>
   </si>
   <si>
-    <t>restando1</t>
-  </si>
-  <si>
-    <t>sumando2</t>
+    <t>restando2</t>
   </si>
   <si>
     <t>valor2</t>
-  </si>
-  <si>
-    <t>restando2</t>
   </si>
   <si>
     <t>valor3</t>
@@ -68,6 +68,9 @@
     <t>tomas</t>
   </si>
   <si>
+    <t>marcos</t>
+  </si>
+  <si>
     <t>dinero</t>
   </si>
 </sst>
@@ -75,7 +78,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -102,6 +105,10 @@
     <font>
       <sz val="10.0"/>
       <color rgb="FF6666FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -191,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -227,10 +234,13 @@
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,7 +483,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -482,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5">
         <v>1.0</v>
@@ -493,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5">
         <v>1.0</v>
@@ -511,13 +521,13 @@
         <f>C2+C3</f>
         <v>2</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="D5" s="14"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="D6" s="14"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="E7" s="15"/>
@@ -1547,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1557,7 +1567,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6">
         <v>2.0</v>
@@ -1569,7 +1579,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6">
         <v>1.0</v>
@@ -1587,7 +1597,7 @@
         <f>C2-C3</f>
         <v>1</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="14"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1609,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -1618,7 +1628,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="6">
         <v>5.0</v>
@@ -1629,7 +1639,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6">
         <v>2.0</v>
@@ -1689,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -1698,7 +1708,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="6">
         <v>5.0</v>
@@ -1720,7 +1730,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5">
         <v>2.0</v>
@@ -1757,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -1771,15 +1781,18 @@
       <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="D2" s="16" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="5">
+        <v>18</v>
+      </c>
+      <c r="C3" s="16">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Base de datos CVS
* Se puede guardar datos
* Se pueden recoger los datos
</commit_message>
<xml_diff>
--- a/TFG/target/excel/excel.xlsx
+++ b/TFG/target/excel/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\Repositorios\Workspace Java\TFG\TFG\target\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFF45C8-B76A-4AA5-9EB4-CC476EF216A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5715CE0E-6888-48CC-9215-F2EEBFA2FEB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{70D779A3-D96A-46DB-9637-FAB903103B3F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>configuracion</t>
   </si>
@@ -48,12 +48,6 @@
   </si>
   <si>
     <t>tomas</t>
-  </si>
-  <si>
-    <t>felipe</t>
-  </si>
-  <si>
-    <t>marcos</t>
   </si>
   <si>
     <t>dinero</t>
@@ -141,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -224,26 +218,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -254,9 +233,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -270,9 +246,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -589,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FEC727-9EBE-4824-9AAA-04B74E38A6A0}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +573,7 @@
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -608,55 +581,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="C3" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7">
-        <v>80</v>
-      </c>
-      <c r="D3" s="7">
-        <v>20</v>
-      </c>
-      <c r="E3" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>5</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>